<commit_message>
Update to stats and figures
</commit_message>
<xml_diff>
--- a/Tables/DIRT20_Bulk_Tables.xlsx
+++ b/Tables/DIRT20_Bulk_Tables.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drkpi\Google Drive\OSU - PhD\Projects\DIRT\DIRT20 Bulk Soil Paper\Tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C61EC4-FE7B-41FE-8F1C-3BFCDC4BC3FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Treatments" sheetId="3" r:id="rId1"/>
     <sheet name="Data table" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="146">
   <si>
     <t>Treatment</t>
   </si>
@@ -177,15 +171,6 @@
     </r>
   </si>
   <si>
-    <t>Bulk density, g cm−3</t>
-  </si>
-  <si>
-    <t>Organic C content, g C m−2</t>
-  </si>
-  <si>
-    <t>Root mass, g m−2</t>
-  </si>
-  <si>
     <t>Control     [CTL]</t>
   </si>
   <si>
@@ -198,9 +183,6 @@
     <t>O-horizon</t>
   </si>
   <si>
-    <t>Surface litter mass, kg m−2</t>
-  </si>
-  <si>
     <t>Soil pH</t>
   </si>
   <si>
@@ -355,6 +337,186 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>16.0 ± 0.7</t>
+  </si>
+  <si>
+    <t>19.6 ± 0.7</t>
+  </si>
+  <si>
+    <t>25.0 ± 1.0</t>
+  </si>
+  <si>
+    <t>16.2 ± 0.9</t>
+  </si>
+  <si>
+    <t>11.7 ± 0.4</t>
+  </si>
+  <si>
+    <t>79 ± 16</t>
+  </si>
+  <si>
+    <t>185 ± 52</t>
+  </si>
+  <si>
+    <t>133 ± 53</t>
+  </si>
+  <si>
+    <t>115 ± 32</t>
+  </si>
+  <si>
+    <t>3.01 ± 0.48</t>
+  </si>
+  <si>
+    <t>3.20 ± 0.66</t>
+  </si>
+  <si>
+    <t>3.06 ± 0.63</t>
+  </si>
+  <si>
+    <t>3.50 ± 0.38</t>
+  </si>
+  <si>
+    <t>3.93 ± 0.41</t>
+  </si>
+  <si>
+    <t>3.29 ± 0.24</t>
+  </si>
+  <si>
+    <t>1.90 ± 0.38</t>
+  </si>
+  <si>
+    <t>2.85 ± 1.01</t>
+  </si>
+  <si>
+    <t>2.07 ± 0.36</t>
+  </si>
+  <si>
+    <t>1.90 ± 0.26</t>
+  </si>
+  <si>
+    <t>2.30 ± 0.09</t>
+  </si>
+  <si>
+    <t>1.79 ± 0.51</t>
+  </si>
+  <si>
+    <t>2.45 ± 0.15</t>
+  </si>
+  <si>
+    <t>1.97 ± 0.22</t>
+  </si>
+  <si>
+    <t>4.35 ± 0.95</t>
+  </si>
+  <si>
+    <t>3.57 ± 0.32</t>
+  </si>
+  <si>
+    <t>3.89 ± 0.32</t>
+  </si>
+  <si>
+    <t>3.83 ± 0.23</t>
+  </si>
+  <si>
+    <t>3.35 ± 0.45</t>
+  </si>
+  <si>
+    <t>2.81 ± 0.53</t>
+  </si>
+  <si>
+    <t>3.24 ± 0.59</t>
+  </si>
+  <si>
+    <t>2.27 ± 0.25</t>
+  </si>
+  <si>
+    <t>2.81 ± 0.74</t>
+  </si>
+  <si>
+    <t>2.70 ± 0.44</t>
+  </si>
+  <si>
+    <t>1.91 ± 0.12</t>
+  </si>
+  <si>
+    <t>2.40 ± 0.62</t>
+  </si>
+  <si>
+    <t>2.50 ± 0.25</t>
+  </si>
+  <si>
+    <t>1.50 ± 0.13</t>
+  </si>
+  <si>
+    <t>2.94 ± 0.40</t>
+  </si>
+  <si>
+    <t>3.77 ± 0.73</t>
+  </si>
+  <si>
+    <t>3.87 ± 1.06</t>
+  </si>
+  <si>
+    <t>2.30 ± 0.55</t>
+  </si>
+  <si>
+    <t>2.16 ± 0.27</t>
+  </si>
+  <si>
+    <t>1.93 ± 0.49</t>
+  </si>
+  <si>
+    <t>2.59 ± 0.46</t>
+  </si>
+  <si>
+    <r>
+      <t>Bulk density, g cm</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>−3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Organic C content, kg C m</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>−2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Root mass, g m</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>−2</t>
+    </r>
   </si>
   <si>
     <r>
@@ -379,43 +541,43 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> g-1 soil day-1</t>
+      <t xml:space="preserve"> g-1 soil day</t>
     </r>
-  </si>
-  <si>
-    <t>16.0 ± 0.7</t>
-  </si>
-  <si>
-    <t>19.6 ± 0.7</t>
-  </si>
-  <si>
-    <t>25.0 ± 1.0</t>
-  </si>
-  <si>
-    <t>16.2 ± 0.9</t>
-  </si>
-  <si>
-    <t>11.7 ± 0.4</t>
-  </si>
-  <si>
-    <t>79 ± 16</t>
-  </si>
-  <si>
-    <t>185 ± 52</t>
-  </si>
-  <si>
-    <t>133 ± 53</t>
-  </si>
-  <si>
-    <t>115 ± 32</t>
+    <r>
+      <rPr>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Surface litter mass, kg m</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>−2</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -579,14 +741,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,6 +765,134 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>14</xdr:col>
+          <xdr:colOff>190500</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$A$1:$C$12" spid="_x0000_s2051"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="6886575" y="285750"/>
+              <a:ext cx="6010275" cy="3590925"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>542925</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:to>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Picture 3"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+              <a:extLst>
+                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
+                  <a14:cameraTool cellRange="$A$1:$H$27" spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="6629400" y="762000"/>
+              <a:ext cx="6029325" cy="5543550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,7 +938,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,26 +971,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,23 +1006,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -925,11 +1181,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,15 +1309,17 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="13"/>
       <c r="C2" s="12"/>
@@ -1087,21 +1345,21 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" s="15" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="15" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>30</v>
@@ -1114,41 +1372,41 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,25 +1414,25 @@
         <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1182,25 +1440,25 @@
         <v>37</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1208,25 +1466,25 @@
         <v>38</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1234,101 +1492,101 @@
         <v>39</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="G11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="H11" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="12" spans="1:8" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="A12" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1336,25 +1594,25 @@
         <v>36</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,25 +1620,25 @@
         <v>37</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,25 +1646,25 @@
         <v>38</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1414,178 +1672,178 @@
         <v>39</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>50</v>
+        <v>134</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>50</v>
+        <v>135</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="J17" s="23"/>
+        <v>140</v>
+      </c>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="A18" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="G19" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="H19" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="A20" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
     </row>
     <row r="21" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E21" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="19" t="s">
-        <v>105</v>
-      </c>
       <c r="G21" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="A22" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="A24" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
     </row>
     <row r="25" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1610,5 +1868,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>